<commit_message>
updated slopes in st curve summary, added viz
</commit_message>
<xml_diff>
--- a/raw data/chla_standardcurve_summary.xlsx
+++ b/raw data/chla_standardcurve_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ant28\OneDrive - Duke University\Documents\Duke University\Research\_HBEF\chla\hbef_chla\raw data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{D4D988AF-7CBE-4A69-98BE-610BCDE92384}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A7555E44-4A6A-4B2D-84AB-D027AA8241A5}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{D4D988AF-7CBE-4A69-98BE-610BCDE92384}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C752D526-741C-4295-9823-69AF2E81D1FF}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" xr2:uid="{16AB7D61-66D5-45EA-8C9A-6D1B57A0A0E8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>CassarTriology</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>slp_id</t>
+  </si>
+  <si>
+    <t>slope_rfu_over_ugL</t>
   </si>
 </sst>
 </file>
@@ -466,15 +469,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882B14C9-DF14-4315-8C7F-5EF98D73C551}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -505,8 +508,11 @@
       <c r="J1" t="s">
         <v>4</v>
       </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -524,7 +530,8 @@
         <v>13</v>
       </c>
       <c r="F2">
-        <v>1.226</v>
+        <f>1/K2</f>
+        <v>0.81566068515497558</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -538,8 +545,11 @@
       <c r="J2" t="s">
         <v>15</v>
       </c>
+      <c r="K2">
+        <v>1.226</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -557,7 +567,8 @@
         <v>3</v>
       </c>
       <c r="F3">
-        <v>0.68200000000000005</v>
+        <f>1/K3</f>
+        <v>1.4662756598240467</v>
       </c>
       <c r="G3">
         <v>574.524</v>
@@ -571,8 +582,11 @@
       <c r="J3" t="s">
         <v>25</v>
       </c>
+      <c r="K3">
+        <v>0.68200000000000005</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -590,7 +604,8 @@
         <v>12</v>
       </c>
       <c r="F4">
-        <v>0.88100000000000001</v>
+        <f>1/K4</f>
+        <v>1.1350737797956867</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -604,8 +619,11 @@
       <c r="J4" t="s">
         <v>25</v>
       </c>
+      <c r="K4">
+        <v>0.88100000000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -637,8 +655,11 @@
       <c r="J5" t="s">
         <v>18</v>
       </c>
+      <c r="K5">
+        <v>1245</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -664,8 +685,11 @@
       <c r="J6" t="s">
         <v>28</v>
       </c>
+      <c r="K6">
+        <v>3547.77</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -683,7 +707,8 @@
         <v>13</v>
       </c>
       <c r="F7">
-        <v>3.83</v>
+        <f>1/K7</f>
+        <v>0.2610966057441253</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -694,8 +719,11 @@
       <c r="J7" t="s">
         <v>23</v>
       </c>
+      <c r="K7">
+        <v>3.83</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -713,7 +741,8 @@
         <v>3</v>
       </c>
       <c r="F8">
-        <v>1.93</v>
+        <f>1/K8</f>
+        <v>0.5181347150259068</v>
       </c>
       <c r="G8">
         <v>2622.7020000000002</v>
@@ -724,8 +753,11 @@
       <c r="J8" t="s">
         <v>24</v>
       </c>
+      <c r="K8">
+        <v>1.93</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -743,7 +775,8 @@
         <v>12</v>
       </c>
       <c r="F9">
-        <v>2.8940000000000001</v>
+        <f>1/K9</f>
+        <v>0.3455425017277125</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -754,8 +787,11 @@
       <c r="J9" t="s">
         <v>24</v>
       </c>
+      <c r="K9">
+        <v>2.8940000000000001</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -781,8 +817,11 @@
       <c r="J10" t="s">
         <v>26</v>
       </c>
+      <c r="K10">
+        <v>5203</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -807,6 +846,9 @@
       </c>
       <c r="J11" t="s">
         <v>27</v>
+      </c>
+      <c r="K11">
+        <v>9716.41</v>
       </c>
     </row>
   </sheetData>
@@ -815,23 +857,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9ceb467c-90f4-4aaa-8637-7333f463bc22" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100132DAEEE68D8F448A2954E31F7D20D2E" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="56f05307a0a85dfa67505d5878c5e62a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9ceb467c-90f4-4aaa-8637-7333f463bc22" xmlns:ns4="8f817a8b-ef11-4508-9b33-f4ee9922bbbe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff4f179617d74248a988119b09e76f78" ns3:_="" ns4:_="">
     <xsd:import namespace="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
@@ -1066,32 +1091,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EA71C4-768B-4955-92EB-267618D50FE2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
-    <ds:schemaRef ds:uri="8f817a8b-ef11-4508-9b33-f4ee9922bbbe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7382369-0E19-4C34-B049-9CAA7E0D97C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9ceb467c-90f4-4aaa-8637-7333f463bc22" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF580C80-A173-4B68-A3B2-84BD2B97E956}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1108,4 +1125,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7382369-0E19-4C34-B049-9CAA7E0D97C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EA71C4-768B-4955-92EB-267618D50FE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8f817a8b-ef11-4508-9b33-f4ee9922bbbe"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update standard curve, add high slope with intercept
</commit_message>
<xml_diff>
--- a/raw data/chla_standardcurve_summary.xlsx
+++ b/raw data/chla_standardcurve_summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ant28\OneDrive - Duke University\Documents\Duke University\Research\_HBEF\chla\hbef_chla\raw data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ant28\OneDrive - Duke University\Documents\Duke University\Research\_HBEF\moss_manuscipt\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{D4D988AF-7CBE-4A69-98BE-610BCDE92384}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C752D526-741C-4295-9823-69AF2E81D1FF}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{D4D988AF-7CBE-4A69-98BE-610BCDE92384}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{5F930FF8-C14F-459B-AF38-DE6A415DE65E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" xr2:uid="{16AB7D61-66D5-45EA-8C9A-6D1B57A0A0E8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>CassarTriology</t>
   </si>
@@ -78,9 +78,6 @@
     <t>cutoff</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>max values in 1000 ug per L</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
   </si>
   <si>
     <t>slp_id</t>
-  </si>
-  <si>
-    <t>slope_rfu_over_ugL</t>
   </si>
 </sst>
 </file>
@@ -469,20 +463,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882B14C9-DF14-4315-8C7F-5EF98D73C551}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
@@ -508,11 +502,8 @@
       <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -530,8 +521,7 @@
         <v>13</v>
       </c>
       <c r="F2">
-        <f>1/K2</f>
-        <v>0.81566068515497558</v>
+        <v>0.81179999999999997</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -545,11 +535,8 @@
       <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="K2">
-        <v>1.226</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -567,26 +554,22 @@
         <v>3</v>
       </c>
       <c r="F3">
-        <f>1/K3</f>
-        <v>1.4662756598240467</v>
+        <v>1.4059999999999999</v>
       </c>
       <c r="G3">
-        <v>574.524</v>
+        <v>-707.27</v>
       </c>
       <c r="H3">
         <v>2023</v>
       </c>
       <c r="I3">
-        <v>0.95899999999999996</v>
+        <v>0.96</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3">
-        <v>0.68200000000000005</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -604,8 +587,7 @@
         <v>12</v>
       </c>
       <c r="F4">
-        <f>1/K4</f>
-        <v>1.1350737797956867</v>
+        <v>1.123</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -617,13 +599,10 @@
         <v>0.98899999999999999</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4">
-        <v>0.88100000000000001</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -643,23 +622,14 @@
       <c r="F5">
         <v>1245</v>
       </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
       <c r="H5">
         <v>2023</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5">
-        <v>1245</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -674,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6">
         <v>3547.77</v>
@@ -683,32 +653,28 @@
         <v>2023</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6">
-        <v>3547.77</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>Cary2022</v>
       </c>
       <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
       <c r="F7">
-        <f>1/K7</f>
-        <v>0.2610966057441253</v>
+        <v>0.26</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -717,66 +683,58 @@
         <v>2022</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7">
-        <v>3.83</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>Cary2022</v>
       </c>
       <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
       </c>
       <c r="F8">
-        <f>1/K8</f>
-        <v>0.5181347150259068</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="G8">
-        <v>2622.7020000000002</v>
+        <v>-1340.12</v>
       </c>
       <c r="H8">
         <v>2022</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8">
-        <v>1.93</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>Cary2022</v>
       </c>
       <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9">
-        <f>1/K9</f>
-        <v>0.3455425017277125</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -785,25 +743,22 @@
         <v>2022</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9">
-        <v>2.8940000000000001</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>Cary2022</v>
       </c>
       <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -815,28 +770,25 @@
         <v>2022</v>
       </c>
       <c r="J10" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10">
-        <v>5203</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>Cary2022</v>
       </c>
       <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
       </c>
       <c r="F11">
         <v>9716.41</v>
@@ -845,10 +797,7 @@
         <v>2022</v>
       </c>
       <c r="J11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11">
-        <v>9716.41</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -857,6 +806,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9ceb467c-90f4-4aaa-8637-7333f463bc22" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100132DAEEE68D8F448A2954E31F7D20D2E" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="56f05307a0a85dfa67505d5878c5e62a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9ceb467c-90f4-4aaa-8637-7333f463bc22" xmlns:ns4="8f817a8b-ef11-4508-9b33-f4ee9922bbbe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff4f179617d74248a988119b09e76f78" ns3:_="" ns4:_="">
     <xsd:import namespace="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
@@ -1091,7 +1048,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1100,15 +1057,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9ceb467c-90f4-4aaa-8637-7333f463bc22" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EA71C4-768B-4955-92EB-267618D50FE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8f817a8b-ef11-4508-9b33-f4ee9922bbbe"/>
+    <ds:schemaRef ds:uri="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF580C80-A173-4B68-A3B2-84BD2B97E956}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1127,27 +1093,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7382369-0E19-4C34-B049-9CAA7E0D97C0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EA71C4-768B-4955-92EB-267618D50FE2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8f817a8b-ef11-4508-9b33-f4ee9922bbbe"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding new standard curve from Duke in 2023
</commit_message>
<xml_diff>
--- a/raw data/chla_standardcurve_summary.xlsx
+++ b/raw data/chla_standardcurve_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ant28\OneDrive - Duke University\Documents\Duke University\Research\_HBEF\moss_manuscipt\data_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ant28\OneDrive - Duke University\Documents\Duke University\Research\_HBEF\chla\hbef_chla\raw data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{D4D988AF-7CBE-4A69-98BE-610BCDE92384}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{5F930FF8-C14F-459B-AF38-DE6A415DE65E}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{D4D988AF-7CBE-4A69-98BE-610BCDE92384}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{51168D27-230B-41AC-87EF-6FB8A59F36A9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" xr2:uid="{16AB7D61-66D5-45EA-8C9A-6D1B57A0A0E8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8360" xr2:uid="{16AB7D61-66D5-45EA-8C9A-6D1B57A0A0E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
   <si>
     <t>CassarTriology</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Duke</t>
   </si>
   <si>
-    <t>standard_curve_2023</t>
-  </si>
-  <si>
     <t>high_full</t>
   </si>
   <si>
@@ -112,6 +109,36 @@
   </si>
   <si>
     <t>slp_id</t>
+  </si>
+  <si>
+    <t>duke_standard_curve_2023</t>
+  </si>
+  <si>
+    <t>duke_standard_curve_2024</t>
+  </si>
+  <si>
+    <t>duke_standard_curve_2025</t>
+  </si>
+  <si>
+    <t>duke_standard_curve_2026</t>
+  </si>
+  <si>
+    <t>duke_standard_curve_2027</t>
+  </si>
+  <si>
+    <t>duke_august_standard_curve_2023</t>
+  </si>
+  <si>
+    <t>BernhardtTriology</t>
+  </si>
+  <si>
+    <t>y/x = rfu/ug per L, high &gt; 1000 ug per L or &gt; 3977rfu</t>
+  </si>
+  <si>
+    <t>y/x = rfu/ug per L, low &lt; 1000 ug per L or &lt;3977rfu</t>
+  </si>
+  <si>
+    <t>DukeAug2023</t>
   </si>
 </sst>
 </file>
@@ -463,49 +490,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882B14C9-DF14-4315-8C7F-5EF98D73C551}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE(C2,H2)</f>
@@ -518,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>0.81179999999999997</v>
@@ -533,12 +560,12 @@
         <v>0.995</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B11" si="0">CONCATENATE(C3,H3)</f>
@@ -551,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>1.4059999999999999</v>
@@ -566,12 +593,12 @@
         <v>0.96</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
@@ -584,7 +611,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>1.123</v>
@@ -599,12 +626,12 @@
         <v>0.98899999999999999</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -617,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>1245</v>
@@ -626,12 +653,12 @@
         <v>2023</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -644,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>3547.77</v>
@@ -653,25 +680,25 @@
         <v>2023</v>
       </c>
       <c r="J6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>Cary2022</v>
       </c>
       <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>0.26</v>
@@ -683,25 +710,25 @@
         <v>2022</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>Cary2022</v>
       </c>
       <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <v>0.51500000000000001</v>
@@ -713,25 +740,25 @@
         <v>2022</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>Cary2022</v>
       </c>
       <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9">
         <v>0.33800000000000002</v>
@@ -743,25 +770,25 @@
         <v>2022</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>Cary2022</v>
       </c>
       <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10">
         <v>5203</v>
@@ -770,25 +797,25 @@
         <v>2022</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>Cary2022</v>
       </c>
       <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
       </c>
       <c r="F11">
         <v>9716.41</v>
@@ -797,6 +824,154 @@
         <v>2022</v>
       </c>
       <c r="J11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>0.2351</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>2023</v>
+      </c>
+      <c r="I12">
+        <v>0.995</v>
+      </c>
+      <c r="J12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>0.437</v>
+      </c>
+      <c r="G13">
+        <v>-877</v>
+      </c>
+      <c r="H13">
+        <v>2023</v>
+      </c>
+      <c r="I13">
+        <v>0.96</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>0.33250000000000002</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>2023</v>
+      </c>
+      <c r="I14">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>3977.04</v>
+      </c>
+      <c r="H15">
+        <v>2023</v>
+      </c>
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>10661.8</v>
+      </c>
+      <c r="H16">
+        <v>2023</v>
+      </c>
+      <c r="J16" t="s">
         <v>26</v>
       </c>
     </row>
@@ -806,11 +981,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9ceb467c-90f4-4aaa-8637-7333f463bc22" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1049,27 +1225,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9ceb467c-90f4-4aaa-8637-7333f463bc22" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EA71C4-768B-4955-92EB-267618D50FE2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7382369-0E19-4C34-B049-9CAA7E0D97C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8f817a8b-ef11-4508-9b33-f4ee9922bbbe"/>
-    <ds:schemaRef ds:uri="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1094,9 +1260,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7382369-0E19-4C34-B049-9CAA7E0D97C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EA71C4-768B-4955-92EB-267618D50FE2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8f817a8b-ef11-4508-9b33-f4ee9922bbbe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
spellcheck & add files
</commit_message>
<xml_diff>
--- a/raw data/chla_standardcurve_summary.xlsx
+++ b/raw data/chla_standardcurve_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ant28\OneDrive - Duke University\Documents\Duke University\Research\_HBEF\chla\hbef_chla\raw data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/athellma_ad_unc_edu/Documents/Documents/Duke University/Research/_HBEF/chla/hbef_chla/raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{D4D988AF-7CBE-4A69-98BE-610BCDE92384}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{51168D27-230B-41AC-87EF-6FB8A59F36A9}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{D4D988AF-7CBE-4A69-98BE-610BCDE92384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EA21AC0-7907-442D-A41C-1B87C5494AC7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8360" xr2:uid="{16AB7D61-66D5-45EA-8C9A-6D1B57A0A0E8}"/>
+    <workbookView xWindow="35730" yWindow="2430" windowWidth="15375" windowHeight="10395" xr2:uid="{16AB7D61-66D5-45EA-8C9A-6D1B57A0A0E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -493,10 +504,13 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -981,12 +995,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9ceb467c-90f4-4aaa-8637-7333f463bc22" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1225,17 +1238,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9ceb467c-90f4-4aaa-8637-7333f463bc22" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7382369-0E19-4C34-B049-9CAA7E0D97C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EA71C4-768B-4955-92EB-267618D50FE2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8f817a8b-ef11-4508-9b33-f4ee9922bbbe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1260,18 +1283,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EA71C4-768B-4955-92EB-267618D50FE2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7382369-0E19-4C34-B049-9CAA7E0D97C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8f817a8b-ef11-4508-9b33-f4ee9922bbbe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added demo data, updated the vignette
</commit_message>
<xml_diff>
--- a/raw data/chla_standardcurve_summary.xlsx
+++ b/raw data/chla_standardcurve_summary.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/athellma_ad_unc_edu/Documents/Documents/Duke University/Research/_HBEF/chla/hbef_chla/raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{D4D988AF-7CBE-4A69-98BE-610BCDE92384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EA21AC0-7907-442D-A41C-1B87C5494AC7}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{D4D988AF-7CBE-4A69-98BE-610BCDE92384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C512C1D-FC2D-4CD2-8182-90DA6EB2101F}"/>
   <bookViews>
-    <workbookView xWindow="35730" yWindow="2430" windowWidth="15375" windowHeight="10395" xr2:uid="{16AB7D61-66D5-45EA-8C9A-6D1B57A0A0E8}"/>
+    <workbookView minimized="1" xWindow="-3230" yWindow="1080" windowWidth="21600" windowHeight="11180" xr2:uid="{16AB7D61-66D5-45EA-8C9A-6D1B57A0A0E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$16</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -202,6 +205,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -501,10 +508,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882B14C9-DF14-4315-8C7F-5EF98D73C551}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection sqref="A1:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -610,7 +618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -757,7 +765,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -905,7 +913,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -990,16 +998,27 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J16" xr:uid="{882B14C9-DF14-4315-8C7F-5EF98D73C551}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="above_detection"/>
+        <filter val="cutoff"/>
+        <filter val="high_full"/>
+        <filter val="low_zero"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9ceb467c-90f4-4aaa-8637-7333f463bc22" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1238,27 +1257,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9ceb467c-90f4-4aaa-8637-7333f463bc22" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EA71C4-768B-4955-92EB-267618D50FE2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7382369-0E19-4C34-B049-9CAA7E0D97C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8f817a8b-ef11-4508-9b33-f4ee9922bbbe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1283,9 +1292,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7382369-0E19-4C34-B049-9CAA7E0D97C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EA71C4-768B-4955-92EB-267618D50FE2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9ceb467c-90f4-4aaa-8637-7333f463bc22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8f817a8b-ef11-4508-9b33-f4ee9922bbbe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>